<commit_message>
Added [ ] in test file
</commit_message>
<xml_diff>
--- a/code/python/data/Gen_Test_Data.xlsx
+++ b/code/python/data/Gen_Test_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentmdh-my.sharepoint.com/personal/dsp14001_student_mdh_se/Documents/-=MDH=--KajviLP/CEL406 - Sensorteknik/Git/polyethylene_sensor/code/python/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dsp14001\OneDrive\OneDrive - Mälardalens högskola\-=MDH=--KajviLP\CEL406 - Sensorteknik\Git\polyethylene_sensor\code\python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0D077BF-420A-4C1E-8616-5177A07BC82F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{F0D077BF-420A-4C1E-8616-5177A07BC82F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{19926779-ABBE-4601-BB40-45D443877A9C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A2DC8D21-FBF5-4E80-AEE7-FC6D363A4224}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A2DC8D21-FBF5-4E80-AEE7-FC6D363A4224}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Values</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>Shifted V_INDX Map</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>]</t>
   </si>
 </sst>
 </file>
@@ -517,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B676B18C-5E60-4ED1-9FDA-A31EE4324B6E}">
   <dimension ref="A1:T65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
@@ -569,7 +575,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P2,15,4))+INDIRECT(ADDRESS(Q2,15,4)))/2</f>
+        <f t="shared" ref="A2:A33" ca="1" si="0">(INDIRECT(ADDRESS(P2,15,4))+INDIRECT(ADDRESS(Q2,15,4)))/2</f>
         <v>3</v>
       </c>
       <c r="B2" s="3"/>
@@ -589,11 +595,11 @@
         <v>3</v>
       </c>
       <c r="P2" s="1">
-        <f>S2+2</f>
+        <f t="shared" ref="P2:P33" si="1">S2+2</f>
         <v>2</v>
       </c>
       <c r="Q2" s="1">
-        <f>T2+2</f>
+        <f t="shared" ref="Q2:Q33" si="2">T2+2</f>
         <v>8</v>
       </c>
       <c r="R2" s="7">
@@ -608,7 +614,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P3,15,4))+INDIRECT(ADDRESS(Q3,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="B3" s="3"/>
@@ -628,11 +634,11 @@
         <v>3</v>
       </c>
       <c r="P3" s="1">
-        <f>S3+2</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q3" s="1">
-        <f>T3+2</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="R3" s="7">
@@ -647,7 +653,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P4,15,4))+INDIRECT(ADDRESS(Q4,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="3"/>
@@ -667,11 +673,11 @@
         <v>3</v>
       </c>
       <c r="P4" s="1">
-        <f>S4+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="Q4" s="1">
-        <f>T4+2</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="R4" s="7">
@@ -686,7 +692,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P5,15,4))+INDIRECT(ADDRESS(Q5,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="B5" s="3"/>
@@ -706,11 +712,11 @@
         <v>3</v>
       </c>
       <c r="P5" s="1">
-        <f>S5+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="Q5" s="1">
-        <f>T5+2</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="R5" s="7">
@@ -725,7 +731,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P6,15,4))+INDIRECT(ADDRESS(Q6,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="B6" s="3"/>
@@ -745,11 +751,11 @@
         <v>3</v>
       </c>
       <c r="P6" s="1">
-        <f>S6+2</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q6" s="1">
-        <f>T6+2</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="R6" s="7">
@@ -764,7 +770,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P7,15,4))+INDIRECT(ADDRESS(Q7,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="B7" s="3"/>
@@ -784,11 +790,11 @@
         <v>3</v>
       </c>
       <c r="P7" s="1">
-        <f>S7+2</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q7" s="1">
-        <f>T7+2</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="R7" s="7">
@@ -803,7 +809,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P8,15,4))+INDIRECT(ADDRESS(Q8,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="B8" s="3"/>
@@ -823,11 +829,11 @@
         <v>3</v>
       </c>
       <c r="P8" s="1">
-        <f>S8+2</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="Q8" s="1">
-        <f>T8+2</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="R8" s="7">
@@ -842,7 +848,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P9,15,4))+INDIRECT(ADDRESS(Q9,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="M9" s="5">
@@ -855,11 +861,11 @@
         <v>3</v>
       </c>
       <c r="P9" s="1">
-        <f>S9+2</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="Q9" s="1">
-        <f>T9+2</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="R9" s="7">
@@ -874,7 +880,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P10,15,4))+INDIRECT(ADDRESS(Q10,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="M10" s="5">
@@ -887,11 +893,11 @@
         <v>3</v>
       </c>
       <c r="P10" s="1">
-        <f>S10+2</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="Q10" s="1">
-        <f>T10+2</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="R10" s="7">
@@ -906,7 +912,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P11,15,4))+INDIRECT(ADDRESS(Q11,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="M11" s="5">
@@ -919,11 +925,11 @@
         <v>3</v>
       </c>
       <c r="P11" s="1">
-        <f>S11+2</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="Q11" s="1">
-        <f>T11+2</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="R11" s="7">
@@ -938,7 +944,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P12,15,4))+INDIRECT(ADDRESS(Q12,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3.55</v>
       </c>
       <c r="M12" s="5">
@@ -951,11 +957,11 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="P12" s="1">
-        <f>S12+2</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="Q12" s="1">
-        <f>T12+2</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="R12" s="7">
@@ -970,7 +976,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P13,15,4))+INDIRECT(ADDRESS(Q13,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3.55</v>
       </c>
       <c r="M13" s="5">
@@ -983,11 +989,11 @@
         <v>3.18</v>
       </c>
       <c r="P13" s="1">
-        <f>S13+2</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="Q13" s="1">
-        <f>T13+2</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="R13" s="7">
@@ -1002,7 +1008,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P14,15,4))+INDIRECT(ADDRESS(Q14,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3.09</v>
       </c>
       <c r="M14" s="5">
@@ -1015,11 +1021,11 @@
         <v>4.3</v>
       </c>
       <c r="P14" s="1">
-        <f>S14+2</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="Q14" s="1">
-        <f>T14+2</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="R14" s="7">
@@ -1034,7 +1040,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P15,15,4))+INDIRECT(ADDRESS(Q15,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3.09</v>
       </c>
       <c r="M15" s="5">
@@ -1047,11 +1053,11 @@
         <v>3</v>
       </c>
       <c r="P15" s="1">
-        <f>S15+2</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="Q15" s="1">
-        <f>T15+2</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="R15" s="7">
@@ -1066,7 +1072,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P16,15,4))+INDIRECT(ADDRESS(Q16,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="M16" s="5">
@@ -1079,11 +1085,11 @@
         <v>3</v>
       </c>
       <c r="P16" s="1">
-        <f>S16+2</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="Q16" s="1">
-        <f>T16+2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="R16" s="7">
@@ -1098,7 +1104,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P17,15,4))+INDIRECT(ADDRESS(Q17,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="M17" s="5">
@@ -1111,11 +1117,11 @@
         <v>3</v>
       </c>
       <c r="P17" s="1">
-        <f>S17+2</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="Q17" s="1">
-        <f>T17+2</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="R17" s="7">
@@ -1130,7 +1136,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P18,15,4))+INDIRECT(ADDRESS(Q18,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="M18" s="5">
@@ -1143,11 +1149,11 @@
         <v>4.08</v>
       </c>
       <c r="P18" s="1">
-        <f>S18+2</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="Q18" s="1">
-        <f>T18+2</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="R18" s="7">
@@ -1162,7 +1168,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P19,15,4))+INDIRECT(ADDRESS(Q19,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3.54</v>
       </c>
       <c r="M19" s="5">
@@ -1175,11 +1181,11 @@
         <v>3</v>
       </c>
       <c r="P19" s="1">
-        <f>S19+2</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="Q19" s="1">
-        <f>T19+2</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="R19" s="7">
@@ -1194,7 +1200,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P20,15,4))+INDIRECT(ADDRESS(Q20,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>4.09</v>
       </c>
       <c r="M20" s="5">
@@ -1207,11 +1213,11 @@
         <v>4.21</v>
       </c>
       <c r="P20" s="1">
-        <f>S20+2</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="Q20" s="1">
-        <f>T20+2</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="R20" s="7">
@@ -1226,7 +1232,7 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P21,15,4))+INDIRECT(ADDRESS(Q21,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>4.1999999999999993</v>
       </c>
       <c r="M21" s="5">
@@ -1239,11 +1245,11 @@
         <v>3.5</v>
       </c>
       <c r="P21" s="1">
-        <f>S21+2</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="Q21" s="1">
-        <f>T21+2</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="R21" s="7">
@@ -1258,7 +1264,7 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P22,15,4))+INDIRECT(ADDRESS(Q22,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3.74</v>
       </c>
       <c r="M22" s="5">
@@ -1271,11 +1277,11 @@
         <v>3</v>
       </c>
       <c r="P22" s="1">
-        <f>S22+2</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="Q22" s="1">
-        <f>T22+2</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="R22" s="7">
@@ -1290,7 +1296,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P23,15,4))+INDIRECT(ADDRESS(Q23,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3.09</v>
       </c>
       <c r="M23" s="5">
@@ -1303,11 +1309,11 @@
         <v>3.05</v>
       </c>
       <c r="P23" s="1">
-        <f>S23+2</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="Q23" s="1">
-        <f>T23+2</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="R23" s="7">
@@ -1322,7 +1328,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P24,15,4))+INDIRECT(ADDRESS(Q24,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="M24" s="5">
@@ -1335,11 +1341,11 @@
         <v>3</v>
       </c>
       <c r="P24" s="1">
-        <f>S24+2</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="Q24" s="1">
-        <f>T24+2</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="R24" s="7">
@@ -1354,7 +1360,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P25,15,4))+INDIRECT(ADDRESS(Q25,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="M25" s="5">
@@ -1367,11 +1373,11 @@
         <v>3</v>
       </c>
       <c r="P25" s="1">
-        <f>S25+2</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="Q25" s="1">
-        <f>T25+2</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="R25" s="7">
@@ -1386,7 +1392,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P26,15,4))+INDIRECT(ADDRESS(Q26,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="M26" s="5">
@@ -1399,11 +1405,11 @@
         <v>3</v>
       </c>
       <c r="P26" s="1">
-        <f>S26+2</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="Q26" s="1">
-        <f>T26+2</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="R26" s="7">
@@ -1418,7 +1424,7 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P27,15,4))+INDIRECT(ADDRESS(Q27,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3.54</v>
       </c>
       <c r="M27" s="5">
@@ -1431,11 +1437,11 @@
         <v>3</v>
       </c>
       <c r="P27" s="1">
-        <f>S27+2</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="Q27" s="1">
-        <f>T27+2</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="R27" s="7">
@@ -1450,7 +1456,7 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P28,15,4))+INDIRECT(ADDRESS(Q28,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>4.1449999999999996</v>
       </c>
       <c r="M28" s="5">
@@ -1463,11 +1469,11 @@
         <v>3</v>
       </c>
       <c r="P28" s="1">
-        <f>S28+2</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="Q28" s="1">
-        <f>T28+2</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="R28" s="7">
@@ -1482,7 +1488,7 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P29,15,4))+INDIRECT(ADDRESS(Q29,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>4.2549999999999999</v>
       </c>
       <c r="M29" s="5">
@@ -1495,11 +1501,11 @@
         <v>3.47</v>
       </c>
       <c r="P29" s="1">
-        <f>S29+2</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="Q29" s="1">
-        <f>T29+2</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="R29" s="7">
@@ -1514,7 +1520,7 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P30,15,4))+INDIRECT(ADDRESS(Q30,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3.6749999999999998</v>
       </c>
       <c r="M30" s="5">
@@ -1527,11 +1533,11 @@
         <v>3</v>
       </c>
       <c r="P30" s="1">
-        <f>S30+2</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="Q30" s="1">
-        <f>T30+2</f>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="R30" s="7">
@@ -1546,7 +1552,7 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P31,15,4))+INDIRECT(ADDRESS(Q31,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3.0249999999999999</v>
       </c>
       <c r="M31" s="5">
@@ -1559,11 +1565,11 @@
         <v>3</v>
       </c>
       <c r="P31" s="1">
-        <f>S31+2</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="Q31" s="1">
-        <f>T31+2</f>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="R31" s="7">
@@ -1578,7 +1584,7 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P32,15,4))+INDIRECT(ADDRESS(Q32,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="M32" s="5">
@@ -1591,11 +1597,11 @@
         <v>3</v>
       </c>
       <c r="P32" s="1">
-        <f>S32+2</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="Q32" s="1">
-        <f>T32+2</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="R32" s="7">
@@ -1610,7 +1616,7 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P33,15,4))+INDIRECT(ADDRESS(Q33,15,4)))/2</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="M33" s="5">
@@ -1623,11 +1629,11 @@
         <v>3</v>
       </c>
       <c r="P33" s="1">
-        <f>S33+2</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="Q33" s="1">
-        <f>T33+2</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="R33" s="7">
@@ -1642,7 +1648,7 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P34,15,4))+INDIRECT(ADDRESS(Q34,15,4)))/2</f>
+        <f t="shared" ref="A34:A65" ca="1" si="3">(INDIRECT(ADDRESS(P34,15,4))+INDIRECT(ADDRESS(Q34,15,4)))/2</f>
         <v>3</v>
       </c>
       <c r="M34" s="5">
@@ -1655,11 +1661,11 @@
         <v>3</v>
       </c>
       <c r="P34" s="1">
-        <f>S34+2</f>
+        <f t="shared" ref="P34:P65" si="4">S34+2</f>
         <v>19</v>
       </c>
       <c r="Q34" s="1">
-        <f>T34+2</f>
+        <f t="shared" ref="Q34:Q65" si="5">T34+2</f>
         <v>26</v>
       </c>
       <c r="R34" s="7">
@@ -1674,7 +1680,7 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P35,15,4))+INDIRECT(ADDRESS(Q35,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3.25</v>
       </c>
       <c r="M35" s="5">
@@ -1687,11 +1693,11 @@
         <v>3</v>
       </c>
       <c r="P35" s="1">
-        <f>S35+2</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="Q35" s="1">
-        <f>T35+2</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="R35" s="7">
@@ -1706,7 +1712,7 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P36,15,4))+INDIRECT(ADDRESS(Q36,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3.855</v>
       </c>
       <c r="M36" s="5">
@@ -1719,11 +1725,11 @@
         <v>3</v>
       </c>
       <c r="P36" s="1">
-        <f>S36+2</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="Q36" s="1">
-        <f>T36+2</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="R36" s="7">
@@ -1738,7 +1744,7 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P37,15,4))+INDIRECT(ADDRESS(Q37,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3.84</v>
       </c>
       <c r="M37" s="5">
@@ -1751,11 +1757,11 @@
         <v>3</v>
       </c>
       <c r="P37" s="1">
-        <f>S37+2</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="Q37" s="1">
-        <f>T37+2</f>
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="R37" s="7">
@@ -1770,7 +1776,7 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P38,15,4))+INDIRECT(ADDRESS(Q38,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3.26</v>
       </c>
       <c r="M38" s="5">
@@ -1783,11 +1789,11 @@
         <v>3</v>
       </c>
       <c r="P38" s="1">
-        <f>S38+2</f>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="Q38" s="1">
-        <f>T38+2</f>
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="R38" s="7">
@@ -1802,7 +1808,7 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P39,15,4))+INDIRECT(ADDRESS(Q39,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3.0249999999999999</v>
       </c>
       <c r="M39" s="5">
@@ -1815,11 +1821,11 @@
         <v>3</v>
       </c>
       <c r="P39" s="1">
-        <f>S39+2</f>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="Q39" s="1">
-        <f>T39+2</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="R39" s="7">
@@ -1834,7 +1840,7 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P40,15,4))+INDIRECT(ADDRESS(Q40,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="M40" s="5">
@@ -1847,11 +1853,11 @@
         <v>3</v>
       </c>
       <c r="P40" s="1">
-        <f>S40+2</f>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="Q40" s="1">
-        <f>T40+2</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="R40" s="7">
@@ -1866,7 +1872,7 @@
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P41,15,4))+INDIRECT(ADDRESS(Q41,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="M41" s="5">
@@ -1879,11 +1885,11 @@
         <v>3</v>
       </c>
       <c r="P41" s="1">
-        <f>S41+2</f>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="Q41" s="1">
-        <f>T41+2</f>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="R41" s="7">
@@ -1898,15 +1904,15 @@
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P42,15,4))+INDIRECT(ADDRESS(Q42,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P42" s="1">
-        <f>S42+2</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="Q42" s="1">
-        <f>T42+2</f>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="R42" s="7">
@@ -1921,15 +1927,15 @@
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P43,15,4))+INDIRECT(ADDRESS(Q43,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3.25</v>
       </c>
       <c r="P43" s="1">
-        <f>S43+2</f>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="Q43" s="1">
-        <f>T43+2</f>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="R43" s="7">
@@ -1944,15 +1950,15 @@
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P44,15,4))+INDIRECT(ADDRESS(Q44,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3.25</v>
       </c>
       <c r="P44" s="1">
-        <f>S44+2</f>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="Q44" s="1">
-        <f>T44+2</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="R44" s="7">
@@ -1967,15 +1973,15 @@
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P45,15,4))+INDIRECT(ADDRESS(Q45,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3.2350000000000003</v>
       </c>
       <c r="P45" s="1">
-        <f>S45+2</f>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="Q45" s="1">
-        <f>T45+2</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="R45" s="7">
@@ -1990,15 +1996,15 @@
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P46,15,4))+INDIRECT(ADDRESS(Q46,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3.2350000000000003</v>
       </c>
       <c r="P46" s="1">
-        <f>S46+2</f>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="Q46" s="1">
-        <f>T46+2</f>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="R46" s="7">
@@ -2013,15 +2019,15 @@
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P47,15,4))+INDIRECT(ADDRESS(Q47,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P47" s="1">
-        <f>S47+2</f>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="Q47" s="1">
-        <f>T47+2</f>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="R47" s="7">
@@ -2036,15 +2042,15 @@
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P48,15,4))+INDIRECT(ADDRESS(Q48,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P48" s="1">
-        <f>S48+2</f>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="Q48" s="1">
-        <f>T48+2</f>
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="R48" s="7">
@@ -2059,15 +2065,15 @@
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P49,15,4))+INDIRECT(ADDRESS(Q49,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P49" s="1">
-        <f>S49+2</f>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="Q49" s="1">
-        <f>T49+2</f>
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="R49" s="7">
@@ -2082,15 +2088,15 @@
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P50,15,4))+INDIRECT(ADDRESS(Q50,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P50" s="1">
-        <f>S50+2</f>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="Q50" s="1">
-        <f>T50+2</f>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="R50" s="7">
@@ -2105,15 +2111,15 @@
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P51,15,4))+INDIRECT(ADDRESS(Q51,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P51" s="1">
-        <f>S51+2</f>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="Q51" s="1">
-        <f>T51+2</f>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="R51" s="7">
@@ -2128,15 +2134,15 @@
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P52,15,4))+INDIRECT(ADDRESS(Q52,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P52" s="1">
-        <f>S52+2</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="Q52" s="1">
-        <f>T52+2</f>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="R52" s="7">
@@ -2151,15 +2157,15 @@
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P53,15,4))+INDIRECT(ADDRESS(Q53,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P53" s="1">
-        <f>S53+2</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="Q53" s="1">
-        <f>T53+2</f>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="R53" s="7">
@@ -2174,15 +2180,15 @@
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P54,15,4))+INDIRECT(ADDRESS(Q54,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P54" s="1">
-        <f>S54+2</f>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="Q54" s="1">
-        <f>T54+2</f>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="R54" s="7">
@@ -2197,15 +2203,15 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P55,15,4))+INDIRECT(ADDRESS(Q55,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P55" s="1">
-        <f>S55+2</f>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="Q55" s="1">
-        <f>T55+2</f>
+        <f t="shared" si="5"/>
         <v>39</v>
       </c>
       <c r="R55" s="7">
@@ -2220,15 +2226,15 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P56,15,4))+INDIRECT(ADDRESS(Q56,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P56" s="1">
-        <f>S56+2</f>
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
       <c r="Q56" s="1">
-        <f>T56+2</f>
+        <f t="shared" si="5"/>
         <v>39</v>
       </c>
       <c r="R56" s="7">
@@ -2243,15 +2249,15 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P57,15,4))+INDIRECT(ADDRESS(Q57,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P57" s="1">
-        <f>S57+2</f>
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
       <c r="Q57" s="1">
-        <f>T57+2</f>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
       <c r="R57" s="7">
@@ -2266,15 +2272,15 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P58,15,4))+INDIRECT(ADDRESS(Q58,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P58" s="1">
-        <f>S58+2</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="Q58" s="1">
-        <f>T58+2</f>
+        <f t="shared" si="5"/>
         <v>37</v>
       </c>
       <c r="R58" s="7">
@@ -2289,15 +2295,15 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P59,15,4))+INDIRECT(ADDRESS(Q59,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P59" s="1">
-        <f>S59+2</f>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="Q59" s="1">
-        <f>T59+2</f>
+        <f t="shared" si="5"/>
         <v>37</v>
       </c>
       <c r="R59" s="7">
@@ -2312,15 +2318,15 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P60,15,4))+INDIRECT(ADDRESS(Q60,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P60" s="1">
-        <f>S60+2</f>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="Q60" s="1">
-        <f>T60+2</f>
+        <f t="shared" si="5"/>
         <v>38</v>
       </c>
       <c r="R60" s="7">
@@ -2335,15 +2341,15 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P61,15,4))+INDIRECT(ADDRESS(Q61,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P61" s="1">
-        <f>S61+2</f>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="Q61" s="1">
-        <f>T61+2</f>
+        <f t="shared" si="5"/>
         <v>38</v>
       </c>
       <c r="R61" s="7">
@@ -2358,15 +2364,15 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P62,15,4))+INDIRECT(ADDRESS(Q62,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P62" s="1">
-        <f>S62+2</f>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="Q62" s="1">
-        <f>T62+2</f>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="R62" s="7">
@@ -2381,15 +2387,15 @@
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P63,15,4))+INDIRECT(ADDRESS(Q63,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P63" s="1">
-        <f>S63+2</f>
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
       <c r="Q63" s="1">
-        <f>T63+2</f>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="R63" s="7">
@@ -2404,15 +2410,15 @@
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P64,15,4))+INDIRECT(ADDRESS(Q64,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P64" s="1">
-        <f>S64+2</f>
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
       <c r="Q64" s="1">
-        <f>T64+2</f>
+        <f t="shared" si="5"/>
         <v>41</v>
       </c>
       <c r="R64" s="7">
@@ -2427,15 +2433,15 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
-        <f ca="1">(INDIRECT(ADDRESS(P65,15,4))+INDIRECT(ADDRESS(Q65,15,4)))/2</f>
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="P65" s="1">
-        <f>S65+2</f>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="Q65" s="1">
-        <f>T65+2</f>
+        <f t="shared" si="5"/>
         <v>41</v>
       </c>
       <c r="R65" s="7">
@@ -2459,396 +2465,406 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8C35FE-230E-4473-833B-13AB8A2F3336}">
-  <dimension ref="A1:A64"/>
+  <dimension ref="A1:A66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <f ca="1">Blad1!A2</f>
-        <v>3</v>
+      <c r="A1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f ca="1">Blad1!A3</f>
+        <f ca="1">Blad1!A2</f>
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f ca="1">Blad1!A4</f>
+        <f ca="1">Blad1!A3</f>
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f ca="1">Blad1!A5</f>
+        <f ca="1">Blad1!A4</f>
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f ca="1">Blad1!A6</f>
+        <f ca="1">Blad1!A5</f>
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f ca="1">Blad1!A7</f>
+        <f ca="1">Blad1!A6</f>
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f ca="1">Blad1!A8</f>
+        <f ca="1">Blad1!A7</f>
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f ca="1">Blad1!A9</f>
+        <f ca="1">Blad1!A8</f>
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f ca="1">Blad1!A10</f>
+        <f ca="1">Blad1!A9</f>
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f ca="1">Blad1!A11</f>
+        <f ca="1">Blad1!A10</f>
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11">
+        <f ca="1">Blad1!A11</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12">
         <f ca="1">Blad1!A12</f>
         <v>3.55</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13">
         <f ca="1">Blad1!A13</f>
         <v>3.55</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14">
         <f ca="1">Blad1!A14</f>
         <v>3.09</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15">
         <f ca="1">Blad1!A15</f>
         <v>3.09</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <f ca="1">Blad1!A16</f>
-        <v>3</v>
-      </c>
-    </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f ca="1">Blad1!A17</f>
+        <f ca="1">Blad1!A16</f>
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f ca="1">Blad1!A18</f>
+        <f ca="1">Blad1!A17</f>
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
+        <f ca="1">Blad1!A18</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
         <f ca="1">Blad1!A19</f>
         <v>3.54</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
         <f ca="1">Blad1!A20</f>
         <v>4.09</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
         <f ca="1">Blad1!A21</f>
         <v>4.1999999999999993</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
         <f ca="1">Blad1!A22</f>
         <v>3.74</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
         <f ca="1">Blad1!A23</f>
         <v>3.09</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <f ca="1">Blad1!A24</f>
-        <v>3</v>
-      </c>
-    </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
-        <f ca="1">Blad1!A25</f>
+        <f ca="1">Blad1!A24</f>
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
-        <f ca="1">Blad1!A26</f>
+        <f ca="1">Blad1!A25</f>
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
+        <f ca="1">Blad1!A26</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
         <f ca="1">Blad1!A27</f>
         <v>3.54</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
         <f ca="1">Blad1!A28</f>
         <v>4.1449999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
         <f ca="1">Blad1!A29</f>
         <v>4.2549999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
         <f ca="1">Blad1!A30</f>
         <v>3.6749999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
         <f ca="1">Blad1!A31</f>
         <v>3.0249999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <f ca="1">Blad1!A32</f>
-        <v>3</v>
-      </c>
-    </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
-        <f ca="1">Blad1!A33</f>
+        <f ca="1">Blad1!A32</f>
         <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33">
-        <f ca="1">Blad1!A34</f>
+        <f ca="1">Blad1!A33</f>
         <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34">
+        <f ca="1">Blad1!A34</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35">
         <f ca="1">Blad1!A35</f>
         <v>3.25</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36">
         <f ca="1">Blad1!A36</f>
         <v>3.855</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37">
         <f ca="1">Blad1!A37</f>
         <v>3.84</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38">
         <f ca="1">Blad1!A38</f>
         <v>3.26</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39">
         <f ca="1">Blad1!A39</f>
         <v>3.0249999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <f ca="1">Blad1!A40</f>
-        <v>3</v>
-      </c>
-    </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40">
-        <f ca="1">Blad1!A41</f>
+        <f ca="1">Blad1!A40</f>
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41">
-        <f ca="1">Blad1!A42</f>
+        <f ca="1">Blad1!A41</f>
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42">
+        <f ca="1">Blad1!A42</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43">
         <f ca="1">Blad1!A43</f>
         <v>3.25</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44">
         <f ca="1">Blad1!A44</f>
         <v>3.25</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45">
         <f ca="1">Blad1!A45</f>
         <v>3.2350000000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46">
         <f ca="1">Blad1!A46</f>
         <v>3.2350000000000003</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <f ca="1">Blad1!A47</f>
-        <v>3</v>
-      </c>
-    </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47">
-        <f ca="1">Blad1!A48</f>
+        <f ca="1">Blad1!A47</f>
         <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48">
-        <f ca="1">Blad1!A49</f>
+        <f ca="1">Blad1!A48</f>
         <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49">
-        <f ca="1">Blad1!A50</f>
+        <f ca="1">Blad1!A49</f>
         <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50">
-        <f ca="1">Blad1!A51</f>
+        <f ca="1">Blad1!A50</f>
         <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51">
-        <f ca="1">Blad1!A52</f>
+        <f ca="1">Blad1!A51</f>
         <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52">
-        <f ca="1">Blad1!A53</f>
+        <f ca="1">Blad1!A52</f>
         <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53">
-        <f ca="1">Blad1!A54</f>
+        <f ca="1">Blad1!A53</f>
         <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54">
-        <f ca="1">Blad1!A55</f>
+        <f ca="1">Blad1!A54</f>
         <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55">
-        <f ca="1">Blad1!A56</f>
+        <f ca="1">Blad1!A55</f>
         <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56">
-        <f ca="1">Blad1!A57</f>
+        <f ca="1">Blad1!A56</f>
         <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57">
-        <f ca="1">Blad1!A58</f>
+        <f ca="1">Blad1!A57</f>
         <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58">
-        <f ca="1">Blad1!A59</f>
+        <f ca="1">Blad1!A58</f>
         <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59">
-        <f ca="1">Blad1!A60</f>
+        <f ca="1">Blad1!A59</f>
         <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60">
-        <f ca="1">Blad1!A61</f>
+        <f ca="1">Blad1!A60</f>
         <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61">
-        <f ca="1">Blad1!A62</f>
+        <f ca="1">Blad1!A61</f>
         <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62">
-        <f ca="1">Blad1!A63</f>
+        <f ca="1">Blad1!A62</f>
         <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63">
-        <f ca="1">Blad1!A64</f>
+        <f ca="1">Blad1!A63</f>
         <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64">
+        <f ca="1">Blad1!A64</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65">
         <f ca="1">Blad1!A65</f>
         <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added matrix and Array in test gen, resaved testArray
</commit_message>
<xml_diff>
--- a/code/python/data/Gen_Test_Data.xlsx
+++ b/code/python/data/Gen_Test_Data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dsp14001\OneDrive\OneDrive - Mälardalens högskola\-=MDH=--KajviLP\CEL406 - Sensorteknik\Git\polyethylene_sensor\code\python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{F0D077BF-420A-4C1E-8616-5177A07BC82F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{19926779-ABBE-4601-BB40-45D443877A9C}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{F0D077BF-420A-4C1E-8616-5177A07BC82F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{22865B30-9B36-47FB-99E5-3EBCC4BDF0C4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A2DC8D21-FBF5-4E80-AEE7-FC6D363A4224}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{A2DC8D21-FBF5-4E80-AEE7-FC6D363A4224}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="Test_Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Blad2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Values</t>
   </si>
@@ -178,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -205,6 +206,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -523,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B676B18C-5E60-4ED1-9FDA-A31EE4324B6E}">
   <dimension ref="A1:T65"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2467,8 +2471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8C35FE-230E-4473-833B-13AB8A2F3336}">
   <dimension ref="A1:A66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2870,4 +2874,229 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD88C0F-87FB-41A5-BB7C-41A58BA8171B}">
+  <dimension ref="A1:A42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
+        <v>3.18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="12">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="12">
+        <v>4.21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="12">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="12">
+        <v>3.47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>